<commit_message>
updated frequency generation for hardware synth
</commit_message>
<xml_diff>
--- a/freq_calcs.xlsx
+++ b/freq_calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MANTY\BlackboardSynth_MANTIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C853F8-E976-4B31-BE70-3018D8384D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD38A36C-A5DE-43A8-9E66-8FB4372FFC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,13 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="29">
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>Down</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="28">
   <si>
     <t>Mult</t>
   </si>
@@ -79,9 +73,6 @@
   </si>
   <si>
     <t>Div:</t>
-  </si>
-  <si>
-    <t>Div/8:</t>
   </si>
   <si>
     <t>Freq.</t>
@@ -146,6 +137,12 @@
   <si>
     <t>Header</t>
   </si>
+  <si>
+    <t>Divis:</t>
+  </si>
+  <si>
+    <t>Div/16:</t>
+  </si>
 </sst>
 </file>
 
@@ -160,12 +157,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -180,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,55 +469,50 @@
   <dimension ref="A1:Q121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
     <col min="15" max="15" width="10.6640625" customWidth="1"/>
     <col min="17" max="17" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
       <c r="N1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -526,15 +525,11 @@
       <c r="C2">
         <v>100000000</v>
       </c>
-      <c r="E2" cm="1">
-        <f t="array" ref="E2:E9">C2/(C3*C4*A2:A9)</f>
-        <v>3516.1744022503517</v>
-      </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I2" t="str">
         <f>_xlfn.CONCAT(H2,G2)</f>
@@ -574,14 +569,11 @@
       <c r="C3">
         <v>316</v>
       </c>
-      <c r="E3">
-        <v>1758.0872011251759</v>
-      </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I3" t="str">
         <f>_xlfn.CONCAT(H3,G3)</f>
@@ -619,14 +611,11 @@
       <c r="C4">
         <v>90</v>
       </c>
-      <c r="E4">
-        <v>879.04360056258793</v>
-      </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(H4,G4)</f>
@@ -661,14 +650,11 @@
       <c r="A5">
         <v>8</v>
       </c>
-      <c r="E5">
-        <v>439.52180028129396</v>
-      </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ref="I5:I68" si="3">_xlfn.CONCAT(H5,G5)</f>
@@ -703,14 +689,11 @@
       <c r="A6">
         <v>16</v>
       </c>
-      <c r="E6">
-        <v>219.76090014064698</v>
-      </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="3"/>
@@ -745,14 +728,11 @@
       <c r="A7">
         <v>32</v>
       </c>
-      <c r="E7">
-        <v>109.88045007032349</v>
-      </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="3"/>
@@ -787,14 +767,11 @@
       <c r="A8">
         <v>64</v>
       </c>
-      <c r="E8">
-        <v>54.940225035161745</v>
-      </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="3"/>
@@ -826,14 +803,11 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="E9" t="e">
-        <v>#DIV/0!</v>
-      </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="3"/>
@@ -869,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="3"/>
@@ -905,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="3"/>
@@ -941,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="3"/>
@@ -974,22 +948,25 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
       <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="3"/>
@@ -1025,22 +1002,22 @@
         <v>0</v>
       </c>
       <c r="B14" cm="1">
-        <f t="array" ref="B14:B25">32.7*(2^(1/12))^A14:A25</f>
-        <v>32.700000000000003</v>
+        <f t="array" ref="B14:B25">261.6*(2^(1/12))^A14:A25</f>
+        <v>261.60000000000002</v>
+      </c>
+      <c r="C14" cm="1">
+        <f t="array" ref="C14:C25">ROUNDUP(C2/(45*B14:B25), 0)</f>
+        <v>8495</v>
       </c>
       <c r="D14" cm="1">
-        <f t="array" ref="D14:D25">ROUNDUP(C2/(720*B14:B25), 0)</f>
-        <v>4248</v>
-      </c>
-      <c r="E14" cm="1">
-        <f t="array" ref="E14:E25">D14:D25/8</f>
-        <v>531</v>
+        <f t="array" ref="D14:D25">C14:C25/16</f>
+        <v>530.9375</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="3"/>
@@ -1076,19 +1053,19 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>34.644443185548958</v>
+        <v>277.15554548439167</v>
+      </c>
+      <c r="C15">
+        <v>8018</v>
       </c>
       <c r="D15">
-        <v>4009</v>
-      </c>
-      <c r="E15">
         <v>501.125</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="3"/>
@@ -1124,19 +1101,19 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>36.704508979716501</v>
+        <v>293.636071837732</v>
+      </c>
+      <c r="C16">
+        <v>7568</v>
       </c>
       <c r="D16">
-        <v>3784</v>
-      </c>
-      <c r="E16">
         <v>473</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="3"/>
@@ -1172,19 +1149,19 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <v>38.887072660588991</v>
+        <v>311.09658128471193</v>
+      </c>
+      <c r="C17">
+        <v>7144</v>
       </c>
       <c r="D17">
-        <v>3572</v>
-      </c>
-      <c r="E17">
         <v>446.5</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="3"/>
@@ -1220,19 +1197,19 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <v>41.199418331562356</v>
+        <v>329.59534665249885</v>
+      </c>
+      <c r="C18">
+        <v>6743</v>
       </c>
       <c r="D18">
-        <v>3372</v>
-      </c>
-      <c r="E18">
-        <v>421.5</v>
+        <v>421.4375</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="3"/>
@@ -1268,19 +1245,19 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>43.649263231360131</v>
+        <v>349.19410585088104</v>
+      </c>
+      <c r="C19">
+        <v>6364</v>
       </c>
       <c r="D19">
-        <v>3182</v>
-      </c>
-      <c r="E19">
         <v>397.75</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="3"/>
@@ -1316,19 +1293,19 @@
         <v>6</v>
       </c>
       <c r="B20">
-        <v>46.244783489600216</v>
+        <v>369.95826791680173</v>
+      </c>
+      <c r="C20">
+        <v>6007</v>
       </c>
       <c r="D20">
-        <v>3004</v>
-      </c>
-      <c r="E20">
-        <v>375.5</v>
+        <v>375.4375</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="3"/>
@@ -1364,19 +1341,19 @@
         <v>7</v>
       </c>
       <c r="B21">
-        <v>48.994641413867498</v>
+        <v>391.95713131093999</v>
+      </c>
+      <c r="C21">
+        <v>5670</v>
       </c>
       <c r="D21">
-        <v>2835</v>
-      </c>
-      <c r="E21">
         <v>354.375</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="3"/>
@@ -1412,19 +1389,19 @@
         <v>8</v>
       </c>
       <c r="B22">
-        <v>51.908014399360134</v>
+        <v>415.26411519488107</v>
+      </c>
+      <c r="C22">
+        <v>5352</v>
       </c>
       <c r="D22">
-        <v>2676</v>
-      </c>
-      <c r="E22">
         <v>334.5</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="3"/>
@@ -1460,19 +1437,19 @@
         <v>9</v>
       </c>
       <c r="B23">
-        <v>54.99462555759294</v>
+        <v>439.95700446074352</v>
+      </c>
+      <c r="C23">
+        <v>5051</v>
       </c>
       <c r="D23">
-        <v>2526</v>
-      </c>
-      <c r="E23">
-        <v>315.75</v>
+        <v>315.6875</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="3"/>
@@ -1508,19 +1485,19 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>58.264776166378198</v>
+        <v>466.11820933102558</v>
+      </c>
+      <c r="C24">
+        <v>4768</v>
       </c>
       <c r="D24">
-        <v>2384</v>
-      </c>
-      <c r="E24">
         <v>298</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="3"/>
@@ -1556,19 +1533,19 @@
         <v>11</v>
       </c>
       <c r="B25">
-        <v>61.729380049382776</v>
+        <v>493.83504039506221</v>
+      </c>
+      <c r="C25">
+        <v>4500</v>
       </c>
       <c r="D25">
-        <v>2250</v>
-      </c>
-      <c r="E25">
         <v>281.25</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="3"/>
@@ -1604,7 +1581,7 @@
         <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="3"/>
@@ -1640,7 +1617,7 @@
         <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="3"/>
@@ -1676,7 +1653,7 @@
         <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="3"/>
@@ -1712,7 +1689,7 @@
         <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="3"/>
@@ -1748,7 +1725,7 @@
         <v>2</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="3"/>
@@ -1784,7 +1761,7 @@
         <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="3"/>
@@ -1820,7 +1797,7 @@
         <v>2</v>
       </c>
       <c r="H32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="3"/>
@@ -1856,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="H33" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="3"/>
@@ -1892,7 +1869,7 @@
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="3"/>
@@ -1928,7 +1905,7 @@
         <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="3"/>
@@ -1964,7 +1941,7 @@
         <v>2</v>
       </c>
       <c r="H36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="3"/>
@@ -2000,7 +1977,7 @@
         <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="3"/>
@@ -2036,7 +2013,7 @@
         <v>3</v>
       </c>
       <c r="H38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="3"/>
@@ -2072,7 +2049,7 @@
         <v>3</v>
       </c>
       <c r="H39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="3"/>
@@ -2108,7 +2085,7 @@
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="3"/>
@@ -2144,7 +2121,7 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="3"/>
@@ -2180,7 +2157,7 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="3"/>
@@ -2216,7 +2193,7 @@
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="3"/>
@@ -2252,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="3"/>
@@ -2288,7 +2265,7 @@
         <v>3</v>
       </c>
       <c r="H45" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="3"/>
@@ -2324,7 +2301,7 @@
         <v>3</v>
       </c>
       <c r="H46" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="3"/>
@@ -2360,7 +2337,7 @@
         <v>3</v>
       </c>
       <c r="H47" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="3"/>
@@ -2396,7 +2373,7 @@
         <v>3</v>
       </c>
       <c r="H48" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="3"/>
@@ -2432,7 +2409,7 @@
         <v>3</v>
       </c>
       <c r="H49" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="3"/>
@@ -2464,23 +2441,23 @@
       </c>
     </row>
     <row r="50" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G50">
+      <c r="G50" s="1">
         <v>4</v>
       </c>
-      <c r="H50" t="s">
-        <v>14</v>
-      </c>
-      <c r="I50" t="str">
+      <c r="H50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" s="1" t="str">
         <f t="shared" si="3"/>
         <v>C4</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="1">
         <v>49</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="1">
         <v>261.60000000000002</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="1">
         <v>530.9208290859666</v>
       </c>
       <c r="M50">
@@ -2504,7 +2481,7 @@
         <v>4</v>
       </c>
       <c r="H51" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="3"/>
@@ -2540,7 +2517,7 @@
         <v>4</v>
       </c>
       <c r="H52" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="3"/>
@@ -2576,7 +2553,7 @@
         <v>4</v>
       </c>
       <c r="H53" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="3"/>
@@ -2612,7 +2589,7 @@
         <v>4</v>
       </c>
       <c r="H54" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="3"/>
@@ -2648,7 +2625,7 @@
         <v>4</v>
       </c>
       <c r="H55" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="3"/>
@@ -2684,7 +2661,7 @@
         <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="3"/>
@@ -2720,7 +2697,7 @@
         <v>4</v>
       </c>
       <c r="H57" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="3"/>
@@ -2756,7 +2733,7 @@
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="3"/>
@@ -2792,7 +2769,7 @@
         <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="3"/>
@@ -2828,7 +2805,7 @@
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="3"/>
@@ -2864,7 +2841,7 @@
         <v>4</v>
       </c>
       <c r="H61" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="3"/>
@@ -2900,7 +2877,7 @@
         <v>5</v>
       </c>
       <c r="H62" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="3"/>
@@ -2936,7 +2913,7 @@
         <v>5</v>
       </c>
       <c r="H63" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="3"/>
@@ -2972,7 +2949,7 @@
         <v>5</v>
       </c>
       <c r="H64" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I64" t="str">
         <f t="shared" si="3"/>
@@ -3008,7 +2985,7 @@
         <v>5</v>
       </c>
       <c r="H65" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" si="3"/>
@@ -3044,7 +3021,7 @@
         <v>5</v>
       </c>
       <c r="H66" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I66" t="str">
         <f t="shared" si="3"/>
@@ -3080,7 +3057,7 @@
         <v>5</v>
       </c>
       <c r="H67" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I67" t="str">
         <f t="shared" si="3"/>
@@ -3116,7 +3093,7 @@
         <v>5</v>
       </c>
       <c r="H68" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I68" t="str">
         <f t="shared" si="3"/>
@@ -3152,7 +3129,7 @@
         <v>5</v>
       </c>
       <c r="H69" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I69" t="str">
         <f t="shared" ref="I69:I121" si="7">_xlfn.CONCAT(H69,G69)</f>
@@ -3188,7 +3165,7 @@
         <v>5</v>
       </c>
       <c r="H70" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" si="7"/>
@@ -3224,7 +3201,7 @@
         <v>5</v>
       </c>
       <c r="H71" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="7"/>
@@ -3260,7 +3237,7 @@
         <v>5</v>
       </c>
       <c r="H72" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="7"/>
@@ -3296,7 +3273,7 @@
         <v>5</v>
       </c>
       <c r="H73" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I73" t="str">
         <f t="shared" si="7"/>
@@ -3332,7 +3309,7 @@
         <v>6</v>
       </c>
       <c r="H74" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I74" t="str">
         <f t="shared" si="7"/>
@@ -3368,7 +3345,7 @@
         <v>6</v>
       </c>
       <c r="H75" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I75" t="str">
         <f t="shared" si="7"/>
@@ -3404,7 +3381,7 @@
         <v>6</v>
       </c>
       <c r="H76" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" si="7"/>
@@ -3440,7 +3417,7 @@
         <v>6</v>
       </c>
       <c r="H77" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="7"/>
@@ -3476,7 +3453,7 @@
         <v>6</v>
       </c>
       <c r="H78" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I78" t="str">
         <f t="shared" si="7"/>
@@ -3512,7 +3489,7 @@
         <v>6</v>
       </c>
       <c r="H79" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" si="7"/>
@@ -3548,7 +3525,7 @@
         <v>6</v>
       </c>
       <c r="H80" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I80" t="str">
         <f t="shared" si="7"/>
@@ -3584,7 +3561,7 @@
         <v>6</v>
       </c>
       <c r="H81" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I81" t="str">
         <f t="shared" si="7"/>
@@ -3620,7 +3597,7 @@
         <v>6</v>
       </c>
       <c r="H82" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I82" t="str">
         <f t="shared" si="7"/>
@@ -3656,7 +3633,7 @@
         <v>6</v>
       </c>
       <c r="H83" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I83" t="str">
         <f t="shared" si="7"/>
@@ -3692,7 +3669,7 @@
         <v>6</v>
       </c>
       <c r="H84" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I84" t="str">
         <f t="shared" si="7"/>
@@ -3728,7 +3705,7 @@
         <v>6</v>
       </c>
       <c r="H85" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I85" t="str">
         <f t="shared" si="7"/>
@@ -3764,7 +3741,7 @@
         <v>7</v>
       </c>
       <c r="H86" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I86" t="str">
         <f t="shared" si="7"/>
@@ -3800,7 +3777,7 @@
         <v>7</v>
       </c>
       <c r="H87" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I87" t="str">
         <f t="shared" si="7"/>
@@ -3836,7 +3813,7 @@
         <v>7</v>
       </c>
       <c r="H88" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I88" t="str">
         <f t="shared" si="7"/>
@@ -3872,7 +3849,7 @@
         <v>7</v>
       </c>
       <c r="H89" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I89" t="str">
         <f t="shared" si="7"/>
@@ -3908,7 +3885,7 @@
         <v>7</v>
       </c>
       <c r="H90" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I90" t="str">
         <f t="shared" si="7"/>
@@ -3944,7 +3921,7 @@
         <v>7</v>
       </c>
       <c r="H91" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I91" t="str">
         <f t="shared" si="7"/>
@@ -3980,7 +3957,7 @@
         <v>7</v>
       </c>
       <c r="H92" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I92" t="str">
         <f t="shared" si="7"/>
@@ -4016,7 +3993,7 @@
         <v>7</v>
       </c>
       <c r="H93" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I93" t="str">
         <f t="shared" si="7"/>
@@ -4052,7 +4029,7 @@
         <v>7</v>
       </c>
       <c r="H94" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I94" t="str">
         <f t="shared" si="7"/>
@@ -4088,7 +4065,7 @@
         <v>7</v>
       </c>
       <c r="H95" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I95" t="str">
         <f t="shared" si="7"/>
@@ -4124,7 +4101,7 @@
         <v>7</v>
       </c>
       <c r="H96" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I96" t="str">
         <f t="shared" si="7"/>
@@ -4160,7 +4137,7 @@
         <v>7</v>
       </c>
       <c r="H97" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I97" t="str">
         <f t="shared" si="7"/>
@@ -4196,7 +4173,7 @@
         <v>8</v>
       </c>
       <c r="H98" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I98" t="str">
         <f t="shared" si="7"/>
@@ -4232,7 +4209,7 @@
         <v>8</v>
       </c>
       <c r="H99" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I99" t="str">
         <f t="shared" si="7"/>
@@ -4268,7 +4245,7 @@
         <v>8</v>
       </c>
       <c r="H100" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I100" t="str">
         <f t="shared" si="7"/>
@@ -4304,7 +4281,7 @@
         <v>8</v>
       </c>
       <c r="H101" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I101" t="str">
         <f t="shared" si="7"/>
@@ -4340,7 +4317,7 @@
         <v>8</v>
       </c>
       <c r="H102" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I102" t="str">
         <f t="shared" si="7"/>
@@ -4376,7 +4353,7 @@
         <v>8</v>
       </c>
       <c r="H103" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I103" t="str">
         <f t="shared" si="7"/>
@@ -4412,7 +4389,7 @@
         <v>8</v>
       </c>
       <c r="H104" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I104" t="str">
         <f t="shared" si="7"/>
@@ -4448,7 +4425,7 @@
         <v>8</v>
       </c>
       <c r="H105" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I105" t="str">
         <f t="shared" si="7"/>
@@ -4484,7 +4461,7 @@
         <v>8</v>
       </c>
       <c r="H106" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I106" t="str">
         <f t="shared" si="7"/>
@@ -4520,7 +4497,7 @@
         <v>8</v>
       </c>
       <c r="H107" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I107" t="str">
         <f t="shared" si="7"/>
@@ -4556,7 +4533,7 @@
         <v>8</v>
       </c>
       <c r="H108" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I108" t="str">
         <f t="shared" si="7"/>
@@ -4592,7 +4569,7 @@
         <v>8</v>
       </c>
       <c r="H109" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I109" t="str">
         <f t="shared" si="7"/>
@@ -4628,7 +4605,7 @@
         <v>9</v>
       </c>
       <c r="H110" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I110" t="str">
         <f t="shared" si="7"/>
@@ -4664,7 +4641,7 @@
         <v>9</v>
       </c>
       <c r="H111" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I111" t="str">
         <f t="shared" si="7"/>
@@ -4700,7 +4677,7 @@
         <v>9</v>
       </c>
       <c r="H112" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I112" t="str">
         <f t="shared" si="7"/>
@@ -4736,7 +4713,7 @@
         <v>9</v>
       </c>
       <c r="H113" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I113" t="str">
         <f t="shared" si="7"/>
@@ -4772,7 +4749,7 @@
         <v>9</v>
       </c>
       <c r="H114" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I114" t="str">
         <f t="shared" si="7"/>
@@ -4808,7 +4785,7 @@
         <v>9</v>
       </c>
       <c r="H115" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I115" t="str">
         <f t="shared" si="7"/>
@@ -4844,7 +4821,7 @@
         <v>9</v>
       </c>
       <c r="H116" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I116" t="str">
         <f t="shared" si="7"/>
@@ -4880,7 +4857,7 @@
         <v>9</v>
       </c>
       <c r="H117" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I117" t="str">
         <f t="shared" si="7"/>
@@ -4916,7 +4893,7 @@
         <v>9</v>
       </c>
       <c r="H118" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I118" t="str">
         <f t="shared" si="7"/>
@@ -4952,7 +4929,7 @@
         <v>9</v>
       </c>
       <c r="H119" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I119" t="str">
         <f t="shared" si="7"/>
@@ -4988,7 +4965,7 @@
         <v>9</v>
       </c>
       <c r="H120" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I120" t="str">
         <f t="shared" si="7"/>
@@ -5024,7 +5001,7 @@
         <v>9</v>
       </c>
       <c r="H121" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I121" t="str">
         <f t="shared" si="7"/>

</xml_diff>